<commit_message>
Enhance full band/split map workflow: add PNG export step and update README with modes and splitter assignments
</commit_message>
<xml_diff>
--- a/Input List/Full Band/Split Map.xlsx
+++ b/Input List/Full Band/Split Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\Full Band\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E3A715-CA80-4AC9-A365-61427C71A02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F651A74-CC90-41CB-9465-61EE0D9F570B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Split Map" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -179,7 +180,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,8 +242,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,8 +300,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -304,21 +331,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -355,69 +367,115 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -429,9 +487,9 @@
   <colors>
     <mruColors>
       <color rgb="FF00E266"/>
+      <color rgb="FF0066FF"/>
       <color rgb="FFA3E0FF"/>
       <color rgb="FFE5F5FF"/>
-      <color rgb="FF0066FF"/>
       <color rgb="FFF2F2F2"/>
       <color rgb="FF99FF99"/>
       <color rgb="FFE2EFDA"/>
@@ -751,7 +809,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,119 +819,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="J1" s="20" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="J1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
     </row>
-    <row r="2" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:17" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="21">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="21">
         <v>3</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="21">
         <v>4</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="22">
         <v>5</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="22">
         <v>6</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="22">
         <v>7</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="22">
         <v>8</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="26">
         <v>9</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="26">
         <v>10</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="26">
         <v>11</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="26">
         <v>12</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="23">
         <v>13</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="23">
         <v>14</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="23">
         <v>15</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="Q2" s="23">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:17" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="7" t="s">
+      <c r="I3" s="2"/>
+      <c r="J3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="17" t="s">
         <v>37</v>
       </c>
       <c r="N3" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="14" t="s">
         <v>9</v>
       </c>
       <c r="P3" s="18" t="s">
@@ -884,110 +942,110 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="15" t="str">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8" t="str">
         <f>"---------------|"</f>
         <v>---------------|</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15" t="s">
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="15"/>
+      <c r="Q4" s="8"/>
     </row>
     <row r="5" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="J5" s="20" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="J5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
     </row>
-    <row r="6" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:17" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
         <v>17</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="25">
         <v>18</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="25">
         <v>19</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="25">
         <v>20</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="27">
         <v>21</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="27">
         <v>22</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="27">
         <v>23</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="27">
         <v>24</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="24">
         <v>25</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="24">
         <v>26</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="24">
         <v>27</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="24">
         <v>28</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="24">
         <v>29</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="24">
         <v>30</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="24">
         <v>31</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q6" s="24">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:17" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="17" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="18" t="s">
@@ -996,105 +1054,105 @@
       <c r="D7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="7" t="s">
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="17" t="s">
         <v>2</v>
       </c>
       <c r="N7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="O7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="P7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" s="20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="16" t="s">
+      <c r="F8" s="9"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16" t="s">
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16" t="s">
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="2"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Update README with splitter assignments and snake tail details
</commit_message>
<xml_diff>
--- a/Input List/Full Band/Split Map.xlsx
+++ b/Input List/Full Band/Split Map.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\Full Band\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\TechnicalDocumentation\Input List\Full Band\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F651A74-CC90-41CB-9465-61EE0D9F570B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F0A2D8-C930-4E22-A947-26C54A4A4F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Split Map" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,30 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Top</t>
   </si>
   <si>
     <t>Bottom</t>
-  </si>
-  <si>
-    <t>Paul
-IEM</t>
-  </si>
-  <si>
-    <t>Kenzi
-IEM</t>
-  </si>
-  <si>
-    <t>Talk
-Back</t>
-  </si>
-  <si>
-    <t>Crowd Left</t>
-  </si>
-  <si>
-    <t>Crowd Right</t>
   </si>
   <si>
     <t>Vocals 1 DSR</t>
@@ -132,12 +113,6 @@
     <t>|--- Bass ---|</t>
   </si>
   <si>
-    <t>| Talkback |</t>
-  </si>
-  <si>
-    <t>|-------------------------------------- Vocals -------------------------------------|</t>
-  </si>
-  <si>
     <t>|---------------------------- Guitars --------------------------|</t>
   </si>
   <si>
@@ -145,20 +120,6 @@
   </si>
   <si>
     <t>The column width needs to be set to 12 so each cell can accurately occupy a single XLR port spacing on the splitter.</t>
-  </si>
-  <si>
-    <t>|----------- Crowd -----------|</t>
-  </si>
-  <si>
-    <t>Chad
-IEM</t>
-  </si>
-  <si>
-    <t>Jessica
-IEM</t>
-  </si>
-  <si>
-    <t>|----------------------------- In-Ear Monitors --------------------------------|</t>
   </si>
   <si>
     <t>|--------------------------------------------------------------- Drums -----------------------------------------------------------------</t>
@@ -172,8 +133,13 @@
 DSL</t>
   </si>
   <si>
-    <t>Billy
-IEM</t>
+    <t>|-------------------------------------------------------- Vocals -------------------------------------------------------|</t>
+  </si>
+  <si>
+    <t>Vocals 6 DCR</t>
+  </si>
+  <si>
+    <t>Vocals 7 DCR</t>
   </si>
 </sst>
 </file>
@@ -266,12 +232,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -318,6 +278,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -399,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -427,6 +393,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -436,47 +441,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -486,6 +453,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF00FF"/>
       <color rgb="FF00E266"/>
       <color rgb="FF0066FF"/>
       <color rgb="FFA3E0FF"/>
@@ -493,7 +461,6 @@
       <color rgb="FFF2F2F2"/>
       <color rgb="FF99FF99"/>
       <color rgb="FFE2EFDA"/>
-      <color rgb="FFFF00FF"/>
       <color rgb="FF00B050"/>
       <color rgb="FF70AD47"/>
     </mruColors>
@@ -809,7 +776,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,131 +786,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="J1" s="12" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="J1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
     </row>
     <row r="2" spans="1:17" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="17">
         <v>2</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="17">
         <v>3</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="17">
         <v>4</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="18">
         <v>5</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="18">
         <v>6</v>
       </c>
-      <c r="G2" s="22">
+      <c r="G2" s="18">
         <v>7</v>
       </c>
-      <c r="H2" s="22">
+      <c r="H2" s="18">
         <v>8</v>
       </c>
-      <c r="J2" s="26">
+      <c r="J2" s="22">
         <v>9</v>
       </c>
-      <c r="K2" s="26">
+      <c r="K2" s="22">
         <v>10</v>
       </c>
-      <c r="L2" s="26">
+      <c r="L2" s="22">
         <v>11</v>
       </c>
-      <c r="M2" s="26">
+      <c r="M2" s="22">
         <v>12</v>
       </c>
-      <c r="N2" s="23">
+      <c r="N2" s="19">
         <v>13</v>
       </c>
-      <c r="O2" s="23">
+      <c r="O2" s="19">
         <v>14</v>
       </c>
-      <c r="P2" s="23">
+      <c r="P2" s="19">
         <v>15</v>
       </c>
-      <c r="Q2" s="23">
+      <c r="Q2" s="19">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="I3" s="2"/>
+      <c r="J3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q3" s="18" t="s">
-        <v>10</v>
+      <c r="K3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="28" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -964,156 +931,138 @@
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
-      <c r="P4" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
     </row>
     <row r="5" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="J5" s="12" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="J5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
     </row>
     <row r="6" spans="1:17" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25">
+      <c r="A6" s="21">
         <v>17</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="21">
         <v>18</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="21">
         <v>19</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="21">
         <v>20</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="23">
         <v>21</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="23">
         <v>22</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="23">
         <v>23</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="23">
         <v>24</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="20">
         <v>25</v>
       </c>
-      <c r="K6" s="24">
+      <c r="K6" s="20">
         <v>26</v>
       </c>
-      <c r="L6" s="24">
+      <c r="L6" s="20">
         <v>27</v>
       </c>
-      <c r="M6" s="24">
+      <c r="M6" s="20">
         <v>28</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="20">
         <v>29</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O6" s="20">
         <v>30</v>
       </c>
-      <c r="P6" s="24">
+      <c r="P6" s="20">
         <v>31</v>
       </c>
-      <c r="Q6" s="24">
+      <c r="Q6" s="20">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>25</v>
+      <c r="A7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
+        <v>19</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="16"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="O7" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="P7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="20" t="s">
-        <v>4</v>
-      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
     </row>
     <row r="8" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="D8" s="9"/>
-      <c r="E8" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="E8" s="27"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
+      <c r="G8" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="H8" s="10"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="O8" s="9"/>
       <c r="P8" s="9"/>
-      <c r="Q8" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="Q8" s="9"/>
     </row>
     <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
@@ -1131,16 +1080,16 @@
       <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="A10" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>